<commit_message>
get_facing tests added but currently failing
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\tsuro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BE38D3-6830-4CDC-9A72-D0D28D299183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F13969-0A17-4100-81BB-9660957B617B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="5700" windowWidth="16680" windowHeight="14715" xr2:uid="{489F35F7-E773-4877-918C-72C3B7E6BF6A}"/>
+    <workbookView xWindow="19650" yWindow="2730" windowWidth="16680" windowHeight="14715" xr2:uid="{489F35F7-E773-4877-918C-72C3B7E6BF6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>tile index</t>
   </si>
@@ -41,6 +41,21 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
@@ -55,12 +70,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,10 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,7 +419,7 @@
   <dimension ref="A1:AA48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,33 +555,37 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
       <c r="Q3">
         <v>1</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
+      <c r="R3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="2"/>
       <c r="T3">
         <v>1</v>
       </c>
@@ -580,33 +606,33 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
       <c r="Q4">
         <v>1</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
       <c r="T4">
         <v>1</v>
       </c>
@@ -677,33 +703,37 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2"/>
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="L6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="2"/>
       <c r="N6">
         <v>1</v>
       </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
       <c r="Q6">
         <v>1</v>
       </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
       <c r="T6">
         <v>1</v>
       </c>
@@ -715,33 +745,33 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
       <c r="N7">
         <v>1</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
       <c r="Q7">
         <v>1</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
       <c r="T7">
         <v>1</v>
       </c>
@@ -794,33 +824,35 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="I9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="2"/>
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
       <c r="N9">
         <v>1</v>
       </c>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
       <c r="Q9">
         <v>1</v>
       </c>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
       <c r="T9">
         <v>1</v>
       </c>
@@ -832,33 +864,33 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
       <c r="K10">
         <v>1</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
       <c r="N10">
         <v>1</v>
       </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
       <c r="Q10">
         <v>1</v>
       </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
       <c r="T10">
         <v>1</v>
       </c>
@@ -911,33 +943,35 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="L12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="2"/>
       <c r="N12">
         <v>1</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
       <c r="Q12">
         <v>1</v>
       </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
       <c r="T12">
         <v>1</v>
       </c>
@@ -949,33 +983,33 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
       <c r="N13">
         <v>1</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
       <c r="Q13">
         <v>1</v>
       </c>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
       <c r="T13">
         <v>1</v>
       </c>
@@ -1028,33 +1062,37 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
       <c r="K15">
         <v>1</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
       <c r="N15">
         <v>1</v>
       </c>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="O15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="2"/>
       <c r="Q15">
         <v>1</v>
       </c>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
       <c r="T15">
         <v>1</v>
       </c>
@@ -1066,33 +1104,33 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16">
         <v>1</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
       <c r="N16">
         <v>1</v>
       </c>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
       <c r="Q16">
         <v>1</v>
       </c>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
       <c r="T16">
         <v>1</v>
       </c>
@@ -1145,33 +1183,37 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="2"/>
       <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
       <c r="N18">
         <v>1</v>
       </c>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
       <c r="Q18">
         <v>1</v>
       </c>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+      <c r="R18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" s="2"/>
       <c r="T18">
         <v>1</v>
       </c>
@@ -1183,33 +1225,33 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
       <c r="K19">
         <v>1</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
       <c r="N19">
         <v>1</v>
       </c>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
       <c r="Q19">
         <v>1</v>
       </c>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
       <c r="T19">
         <v>1</v>
       </c>
@@ -1301,6 +1343,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
@@ -1309,26 +1365,74 @@
         <f>MOD(A30,3)</f>
         <v>0</v>
       </c>
+      <c r="C30">
+        <f>B30-1</f>
+        <v>-1</v>
+      </c>
+      <c r="D30">
+        <f>B30+1</f>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f>ABS(B30-6)</f>
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <f>ABS(B30-8)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>1</v>
       </c>
       <c r="B31">
         <f t="shared" ref="B31:B48" si="0">MOD(A31,3)</f>
         <v>1</v>
       </c>
+      <c r="C31" s="1">
+        <f t="shared" ref="C31:C48" si="1">B31-1</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" ref="D31:D48" si="2">B31+1</f>
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" ref="E31:E48" si="3">ABS(B31-6)</f>
+        <v>5</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" ref="F31:F48" si="4">ABS(B31-8)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>2</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1336,26 +1440,74 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>4</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="C34" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>5</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6</v>
       </c>
@@ -1363,26 +1515,74 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>7</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="C37" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>8</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9</v>
       </c>
@@ -1390,26 +1590,74 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>10</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="C40" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>11</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12</v>
       </c>
@@ -1417,26 +1665,74 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>13</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="C43" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>14</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>15</v>
       </c>
@@ -1444,26 +1740,74 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>16</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="C46" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>17</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>18</v>
       </c>
@@ -1471,9 +1815,49 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="R18:S19"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="R15:S16"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="O18:P19"/>
+    <mergeCell ref="R12:S13"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="R9:S10"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="O12:P13"/>
     <mergeCell ref="R6:S7"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="F3:G4"/>
@@ -1486,30 +1870,6 @@
     <mergeCell ref="I6:J7"/>
     <mergeCell ref="L6:M7"/>
     <mergeCell ref="O6:P7"/>
-    <mergeCell ref="R12:S13"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="O9:P10"/>
-    <mergeCell ref="R9:S10"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="O12:P13"/>
-    <mergeCell ref="R18:S19"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="R15:S16"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="O18:P19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>